<commit_message>
move motor to cavity under plate
</commit_message>
<xml_diff>
--- a/CAW.xlsx
+++ b/CAW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Desktop\ball_on_beam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE134C90-A66C-4A41-AE81-683F2AB5D49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF86E22A-043F-410B-B294-D4E853772A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="6966" windowWidth="11688" windowHeight="7578" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2994" yWindow="5142" windowWidth="11688" windowHeight="7578" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -536,7 +536,7 @@
       <c r="D7" s="1">
         <v>6.99</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -577,6 +577,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E8" r:id="rId1" xr:uid="{F2EBCD99-D5D1-4B3B-AA92-99CFB77CFCC0}"/>
+    <hyperlink ref="E7" r:id="rId2" xr:uid="{84B6E2EB-DDDA-4F65-9772-A64E3C60E7B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add sensor and nuts and bolts
</commit_message>
<xml_diff>
--- a/CAW.xlsx
+++ b/CAW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Desktop\ball_on_beam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6337E264-1D50-49EF-847B-889911C453ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561362A2-C104-42E4-9213-622B1A6D991A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-78" yWindow="0" windowWidth="11676" windowHeight="14478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Cost Accounting Worksheet</t>
   </si>
@@ -134,30 +134,6 @@
     <t>https://www.adafruit.com/product/550?gQT=1</t>
   </si>
   <si>
-    <t>https://www.adafruit.com/product/3316</t>
-  </si>
-  <si>
-    <t>Adafruit VL6180X Time of Flight Distance Ranging Sensor</t>
-  </si>
-  <si>
-    <t>Panel Mount 10K potentiometer (Breadboard Friendly) - 10K Linear</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/562</t>
-  </si>
-  <si>
-    <t>Anodized Aluminum Machined Knob - Black - 20mm Diameter</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/5527</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/4219</t>
-  </si>
-  <si>
-    <t>Slide Potentiometer with Knob - 75mm Long - 10KΩ</t>
-  </si>
-  <si>
     <t>Rugged Metal On/Off Switch with White LED Ring - 16mm</t>
   </si>
   <si>
@@ -174,6 +150,24 @@
   </si>
   <si>
     <t>Arcade Button Quick-Connect Wire Pairs - 0.11" (10 pack)</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/5396</t>
+  </si>
+  <si>
+    <t>Adafruit VL53L4CD Time of Flight Distance Sensor</t>
+  </si>
+  <si>
+    <t>High-Strength 316 Stainless Steel Socket Head Screw, M4 x 0.70 mm Thread, 10 mm Long</t>
+  </si>
+  <si>
+    <t>High-Strength Steel Nylon-Insert Locknut Class 10, Zinc Plated, M4 x 0.7 mm Thread, 5 mm High</t>
+  </si>
+  <si>
+    <t>Medium-Strength Steel Nylon-Insert Locknut Class 8, Zinc-Plated, M2 x 0.4 mm Thread Size</t>
+  </si>
+  <si>
+    <t>High-Strength 316 Stainless Steel Socket Head Screw, M2 x 0.40 mm Thread, 8 mm Long</t>
   </si>
 </sst>
 </file>
@@ -515,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -587,7 +581,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E16" si="0">D5*C5</f>
+        <f t="shared" ref="E5:E14" si="0">D5*C5</f>
         <v>2.1800000000000002</v>
       </c>
       <c r="F5" t="s">
@@ -719,7 +713,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B12">
         <v>917</v>
@@ -735,12 +729,12 @@
         <v>4.95</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B13">
         <v>558</v>
@@ -756,131 +750,133 @@
         <v>14.850000000000001</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>5396</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>14.95</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>29.9</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0.95</v>
+      </c>
+      <c r="E15" s="1">
+        <f>D15*C15</f>
+        <v>0.95</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4.95</v>
+      </c>
+      <c r="E16" s="1">
+        <f>D16*C16</f>
+        <v>4.95</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17">
+        <v>4</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="1">
         <f>SUM(E4:E18)</f>
-        <v>62.480000000000011</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>0.95</v>
-      </c>
-      <c r="E26" s="1">
-        <f>D26*C26</f>
-        <v>0.95</v>
-      </c>
-      <c r="F26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" s="1">
-        <v>13.95</v>
-      </c>
-      <c r="E27" s="1">
-        <f>D27*C27</f>
-        <v>27.9</v>
-      </c>
-      <c r="F27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="E28" s="1">
-        <f>D28*C28</f>
-        <v>2.8499999999999996</v>
-      </c>
-      <c r="F28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2.95</v>
-      </c>
-      <c r="E29" s="1">
-        <f>D29*C29</f>
-        <v>8.8500000000000014</v>
-      </c>
-      <c r="F29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2.95</v>
-      </c>
-      <c r="E30" s="1">
-        <f>D30*C30</f>
-        <v>2.95</v>
-      </c>
-      <c r="F30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" t="s">
-        <v>44</v>
-      </c>
+        <v>98.280000000000015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1" xr:uid="{F2EBCD99-D5D1-4B3B-AA92-99CFB77CFCC0}"/>
     <hyperlink ref="F7" r:id="rId2" xr:uid="{84B6E2EB-DDDA-4F65-9772-A64E3C60E7B2}"/>
     <hyperlink ref="F13" r:id="rId3" xr:uid="{56C1AAAD-8D9A-4DA5-9665-B609B7178CF6}"/>
+    <hyperlink ref="F14" r:id="rId4" xr:uid="{C8F5265F-C4FC-4B47-A191-882872824E5F}"/>
+    <hyperlink ref="F16" r:id="rId5" xr:uid="{B1268CA3-68D3-4790-9FF0-85B7569ADB7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>